<commit_message>
updated outputs-HGR-r202-archive3 and lock
</commit_message>
<xml_diff>
--- a/outputs-HGR-r202-archive3/c__Coriobacteriia.xlsx
+++ b/outputs-HGR-r202-archive3/c__Coriobacteriia.xlsx
@@ -447,17 +447,17 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>prediction</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>rejection-f</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>max</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>prediction</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>rejection-f</t>
         </is>
       </c>
     </row>
@@ -470,18 +470,18 @@
       <c r="B2" t="n">
         <v>43141.03612922395</v>
       </c>
-      <c r="C2" t="n">
-        <v>43141.03612922395</v>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>o__Coriobacteriales</t>
+        </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
           <t>o__Coriobacteriales</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>o__Coriobacteriales</t>
-        </is>
+      <c r="E2" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -493,18 +493,18 @@
       <c r="B3" t="n">
         <v>120075.8643859128</v>
       </c>
-      <c r="C3" t="n">
-        <v>120075.8643859128</v>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>o__Coriobacteriales</t>
+        </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
           <t>o__Coriobacteriales</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>o__Coriobacteriales</t>
-        </is>
+      <c r="E3" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -516,18 +516,18 @@
       <c r="B4" t="n">
         <v>47309.6101292944</v>
       </c>
-      <c r="C4" t="n">
-        <v>47309.6101292944</v>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>o__Coriobacteriales</t>
+        </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
           <t>o__Coriobacteriales</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>o__Coriobacteriales</t>
-        </is>
+      <c r="E4" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -539,18 +539,18 @@
       <c r="B5" t="n">
         <v>49169.4427639097</v>
       </c>
-      <c r="C5" t="n">
-        <v>49169.4427639097</v>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>o__Coriobacteriales</t>
+        </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
           <t>o__Coriobacteriales</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>o__Coriobacteriales</t>
-        </is>
+      <c r="E5" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="6">
@@ -562,18 +562,18 @@
       <c r="B6" t="n">
         <v>131765.9075807838</v>
       </c>
-      <c r="C6" t="n">
-        <v>131765.9075807838</v>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>o__Coriobacteriales</t>
+        </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
           <t>o__Coriobacteriales</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>o__Coriobacteriales</t>
-        </is>
+      <c r="E6" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="7">
@@ -585,18 +585,18 @@
       <c r="B7" t="n">
         <v>96259.59930645699</v>
       </c>
-      <c r="C7" t="n">
-        <v>96259.59930645699</v>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>o__Coriobacteriales</t>
+        </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
           <t>o__Coriobacteriales</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>o__Coriobacteriales</t>
-        </is>
+      <c r="E7" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="8">
@@ -608,18 +608,18 @@
       <c r="B8" t="n">
         <v>95688.67098190574</v>
       </c>
-      <c r="C8" t="n">
-        <v>95688.67098190574</v>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>o__Coriobacteriales</t>
+        </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
           <t>o__Coriobacteriales</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>o__Coriobacteriales</t>
-        </is>
+      <c r="E8" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="9">
@@ -631,18 +631,18 @@
       <c r="B9" t="n">
         <v>93266.57600363872</v>
       </c>
-      <c r="C9" t="n">
-        <v>93266.57600363872</v>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>o__Coriobacteriales</t>
+        </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
           <t>o__Coriobacteriales</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>o__Coriobacteriales</t>
-        </is>
+      <c r="E9" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="10">
@@ -654,18 +654,18 @@
       <c r="B10" t="n">
         <v>93171.38466286469</v>
       </c>
-      <c r="C10" t="n">
-        <v>93171.38466286469</v>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>o__Coriobacteriales</t>
+        </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
           <t>o__Coriobacteriales</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>o__Coriobacteriales</t>
-        </is>
+      <c r="E10" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="11">
@@ -677,18 +677,18 @@
       <c r="B11" t="n">
         <v>91717.23241513476</v>
       </c>
-      <c r="C11" t="n">
-        <v>91717.23241513476</v>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>o__Coriobacteriales</t>
+        </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
           <t>o__Coriobacteriales</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>o__Coriobacteriales</t>
-        </is>
+      <c r="E11" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="12">
@@ -700,18 +700,18 @@
       <c r="B12" t="n">
         <v>92441.47801882646</v>
       </c>
-      <c r="C12" t="n">
-        <v>92441.47801882646</v>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>o__Coriobacteriales</t>
+        </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
           <t>o__Coriobacteriales</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>o__Coriobacteriales</t>
-        </is>
+      <c r="E12" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="13">
@@ -723,18 +723,18 @@
       <c r="B13" t="n">
         <v>94240.51658987721</v>
       </c>
-      <c r="C13" t="n">
-        <v>94240.51658987721</v>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>o__Coriobacteriales</t>
+        </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
           <t>o__Coriobacteriales</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>o__Coriobacteriales</t>
-        </is>
+      <c r="E13" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="14">
@@ -746,18 +746,18 @@
       <c r="B14" t="n">
         <v>94898.47214745055</v>
       </c>
-      <c r="C14" t="n">
-        <v>94898.47214745055</v>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>o__Coriobacteriales</t>
+        </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
           <t>o__Coriobacteriales</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>o__Coriobacteriales</t>
-        </is>
+      <c r="E14" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="15">
@@ -769,18 +769,18 @@
       <c r="B15" t="n">
         <v>90132.56130785077</v>
       </c>
-      <c r="C15" t="n">
-        <v>90132.56130785077</v>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>o__Coriobacteriales</t>
+        </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
           <t>o__Coriobacteriales</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>o__Coriobacteriales</t>
-        </is>
+      <c r="E15" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="16">
@@ -792,18 +792,18 @@
       <c r="B16" t="n">
         <v>41991.312170301</v>
       </c>
-      <c r="C16" t="n">
-        <v>41991.312170301</v>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>o__Coriobacteriales</t>
+        </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
           <t>o__Coriobacteriales</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>o__Coriobacteriales</t>
-        </is>
+      <c r="E16" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="17">
@@ -815,18 +815,18 @@
       <c r="B17" t="n">
         <v>87864.60216703171</v>
       </c>
-      <c r="C17" t="n">
-        <v>87864.60216703171</v>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>o__Coriobacteriales</t>
+        </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
           <t>o__Coriobacteriales</t>
         </is>
       </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>o__Coriobacteriales</t>
-        </is>
+      <c r="E17" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="18">
@@ -838,18 +838,18 @@
       <c r="B18" t="n">
         <v>87490.49213624472</v>
       </c>
-      <c r="C18" t="n">
-        <v>87490.49213624472</v>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>o__Coriobacteriales</t>
+        </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
           <t>o__Coriobacteriales</t>
         </is>
       </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>o__Coriobacteriales</t>
-        </is>
+      <c r="E18" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="19">
@@ -861,18 +861,18 @@
       <c r="B19" t="n">
         <v>46117.67828512657</v>
       </c>
-      <c r="C19" t="n">
-        <v>46117.67828512657</v>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>o__Coriobacteriales</t>
+        </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
           <t>o__Coriobacteriales</t>
         </is>
       </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>o__Coriobacteriales</t>
-        </is>
+      <c r="E19" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="20">
@@ -884,18 +884,18 @@
       <c r="B20" t="n">
         <v>86698.70271543616</v>
       </c>
-      <c r="C20" t="n">
-        <v>86698.70271543616</v>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>o__Coriobacteriales</t>
+        </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
           <t>o__Coriobacteriales</t>
         </is>
       </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>o__Coriobacteriales</t>
-        </is>
+      <c r="E20" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="21">
@@ -907,18 +907,18 @@
       <c r="B21" t="n">
         <v>124645.0909236251</v>
       </c>
-      <c r="C21" t="n">
-        <v>124645.0909236251</v>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>o__Coriobacteriales</t>
+        </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
           <t>o__Coriobacteriales</t>
         </is>
       </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>o__Coriobacteriales</t>
-        </is>
+      <c r="E21" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="22">
@@ -930,18 +930,18 @@
       <c r="B22" t="n">
         <v>129359.0376472158</v>
       </c>
-      <c r="C22" t="n">
-        <v>129359.0376472158</v>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>o__Coriobacteriales</t>
+        </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
           <t>o__Coriobacteriales</t>
         </is>
       </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>o__Coriobacteriales</t>
-        </is>
+      <c r="E22" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="23">
@@ -953,18 +953,18 @@
       <c r="B23" t="n">
         <v>88918.73375183204</v>
       </c>
-      <c r="C23" t="n">
-        <v>88918.73375183204</v>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>o__Coriobacteriales</t>
+        </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
           <t>o__Coriobacteriales</t>
         </is>
       </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>o__Coriobacteriales</t>
-        </is>
+      <c r="E23" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="24">
@@ -976,18 +976,18 @@
       <c r="B24" t="n">
         <v>94368.46589565495</v>
       </c>
-      <c r="C24" t="n">
-        <v>94368.46589565495</v>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>o__Coriobacteriales</t>
+        </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
           <t>o__Coriobacteriales</t>
         </is>
       </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>o__Coriobacteriales</t>
-        </is>
+      <c r="E24" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="25">
@@ -999,18 +999,18 @@
       <c r="B25" t="n">
         <v>93846.77019192964</v>
       </c>
-      <c r="C25" t="n">
-        <v>93846.77019192964</v>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>o__Coriobacteriales</t>
+        </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
           <t>o__Coriobacteriales</t>
         </is>
       </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>o__Coriobacteriales</t>
-        </is>
+      <c r="E25" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="26">
@@ -1022,18 +1022,18 @@
       <c r="B26" t="n">
         <v>93871.0323252439</v>
       </c>
-      <c r="C26" t="n">
-        <v>93871.0323252439</v>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>o__Coriobacteriales</t>
+        </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
           <t>o__Coriobacteriales</t>
         </is>
       </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>o__Coriobacteriales</t>
-        </is>
+      <c r="E26" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="27">
@@ -1045,18 +1045,18 @@
       <c r="B27" t="n">
         <v>129085.8525149121</v>
       </c>
-      <c r="C27" t="n">
-        <v>129085.8525149121</v>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>o__Coriobacteriales</t>
+        </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
           <t>o__Coriobacteriales</t>
         </is>
       </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>o__Coriobacteriales</t>
-        </is>
+      <c r="E27" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="28">
@@ -1068,18 +1068,18 @@
       <c r="B28" t="n">
         <v>120911.4631066897</v>
       </c>
-      <c r="C28" t="n">
-        <v>120911.4631066897</v>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>o__Coriobacteriales</t>
+        </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
           <t>o__Coriobacteriales</t>
         </is>
       </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>o__Coriobacteriales</t>
-        </is>
+      <c r="E28" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="29">
@@ -1091,18 +1091,18 @@
       <c r="B29" t="n">
         <v>128349.729816296</v>
       </c>
-      <c r="C29" t="n">
-        <v>128349.729816296</v>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>o__Coriobacteriales</t>
+        </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
           <t>o__Coriobacteriales</t>
         </is>
       </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>o__Coriobacteriales</t>
-        </is>
+      <c r="E29" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="30">
@@ -1114,18 +1114,18 @@
       <c r="B30" t="n">
         <v>130594.9432909676</v>
       </c>
-      <c r="C30" t="n">
-        <v>130594.9432909676</v>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>o__Coriobacteriales</t>
+        </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
           <t>o__Coriobacteriales</t>
         </is>
       </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>o__Coriobacteriales</t>
-        </is>
+      <c r="E30" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="31">
@@ -1137,18 +1137,18 @@
       <c r="B31" t="n">
         <v>127611.3990207982</v>
       </c>
-      <c r="C31" t="n">
-        <v>127611.3990207982</v>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>o__Coriobacteriales</t>
+        </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
           <t>o__Coriobacteriales</t>
         </is>
       </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>o__Coriobacteriales</t>
-        </is>
+      <c r="E31" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="32">
@@ -1160,18 +1160,18 @@
       <c r="B32" t="n">
         <v>130400.9715894998</v>
       </c>
-      <c r="C32" t="n">
-        <v>130400.9715894998</v>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>o__Coriobacteriales</t>
+        </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
           <t>o__Coriobacteriales</t>
         </is>
       </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t>o__Coriobacteriales</t>
-        </is>
+      <c r="E32" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="33">
@@ -1183,18 +1183,18 @@
       <c r="B33" t="n">
         <v>44324.71608632716</v>
       </c>
-      <c r="C33" t="n">
-        <v>44324.71608632716</v>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>o__Coriobacteriales</t>
+        </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
           <t>o__Coriobacteriales</t>
         </is>
       </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>o__Coriobacteriales</t>
-        </is>
+      <c r="E33" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="34">
@@ -1206,18 +1206,18 @@
       <c r="B34" t="n">
         <v>134079.661129615</v>
       </c>
-      <c r="C34" t="n">
-        <v>134079.661129615</v>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>o__Coriobacteriales</t>
+        </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
           <t>o__Coriobacteriales</t>
         </is>
       </c>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t>o__Coriobacteriales</t>
-        </is>
+      <c r="E34" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="35">
@@ -1229,18 +1229,18 @@
       <c r="B35" t="n">
         <v>133293.9174786279</v>
       </c>
-      <c r="C35" t="n">
-        <v>133293.9174786279</v>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>o__Coriobacteriales</t>
+        </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
           <t>o__Coriobacteriales</t>
         </is>
       </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>o__Coriobacteriales</t>
-        </is>
+      <c r="E35" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="36">
@@ -1252,18 +1252,18 @@
       <c r="B36" t="n">
         <v>129013.5754206728</v>
       </c>
-      <c r="C36" t="n">
-        <v>129013.5754206728</v>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>o__Coriobacteriales</t>
+        </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
           <t>o__Coriobacteriales</t>
         </is>
       </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>o__Coriobacteriales</t>
-        </is>
+      <c r="E36" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="37">
@@ -1275,18 +1275,18 @@
       <c r="B37" t="n">
         <v>77276.61349156911</v>
       </c>
-      <c r="C37" t="n">
-        <v>77276.61349156911</v>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>o__Coriobacteriales</t>
+        </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
           <t>o__Coriobacteriales</t>
         </is>
       </c>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>o__Coriobacteriales</t>
-        </is>
+      <c r="E37" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="38">
@@ -1298,18 +1298,18 @@
       <c r="B38" t="n">
         <v>140775.1748826397</v>
       </c>
-      <c r="C38" t="n">
-        <v>140775.1748826397</v>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>o__Coriobacteriales</t>
+        </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
           <t>o__Coriobacteriales</t>
         </is>
       </c>
-      <c r="E38" t="inlineStr">
-        <is>
-          <t>o__Coriobacteriales</t>
-        </is>
+      <c r="E38" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="39">
@@ -1321,18 +1321,18 @@
       <c r="B39" t="n">
         <v>123892.2378844079</v>
       </c>
-      <c r="C39" t="n">
-        <v>123892.2378844079</v>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>o__Coriobacteriales</t>
+        </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
           <t>o__Coriobacteriales</t>
         </is>
       </c>
-      <c r="E39" t="inlineStr">
-        <is>
-          <t>o__Coriobacteriales</t>
-        </is>
+      <c r="E39" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="40">
@@ -1344,18 +1344,18 @@
       <c r="B40" t="n">
         <v>133912.2072386561</v>
       </c>
-      <c r="C40" t="n">
-        <v>133912.2072386561</v>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>o__Coriobacteriales</t>
+        </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
           <t>o__Coriobacteriales</t>
         </is>
       </c>
-      <c r="E40" t="inlineStr">
-        <is>
-          <t>o__Coriobacteriales</t>
-        </is>
+      <c r="E40" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="41">
@@ -1367,18 +1367,18 @@
       <c r="B41" t="n">
         <v>90378.84737191322</v>
       </c>
-      <c r="C41" t="n">
-        <v>90378.84737191322</v>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>o__Coriobacteriales</t>
+        </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
           <t>o__Coriobacteriales</t>
         </is>
       </c>
-      <c r="E41" t="inlineStr">
-        <is>
-          <t>o__Coriobacteriales</t>
-        </is>
+      <c r="E41" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="42">
@@ -1390,18 +1390,18 @@
       <c r="B42" t="n">
         <v>89861.42041709919</v>
       </c>
-      <c r="C42" t="n">
-        <v>89861.42041709919</v>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>o__Coriobacteriales</t>
+        </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
           <t>o__Coriobacteriales</t>
         </is>
       </c>
-      <c r="E42" t="inlineStr">
-        <is>
-          <t>o__Coriobacteriales</t>
-        </is>
+      <c r="E42" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="43">
@@ -1413,18 +1413,18 @@
       <c r="B43" t="n">
         <v>135191.3399515467</v>
       </c>
-      <c r="C43" t="n">
-        <v>135191.3399515467</v>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>o__Coriobacteriales</t>
+        </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
           <t>o__Coriobacteriales</t>
         </is>
       </c>
-      <c r="E43" t="inlineStr">
-        <is>
-          <t>o__Coriobacteriales</t>
-        </is>
+      <c r="E43" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="44">
@@ -1436,18 +1436,18 @@
       <c r="B44" t="n">
         <v>92229.6900611392</v>
       </c>
-      <c r="C44" t="n">
-        <v>92229.6900611392</v>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>o__Coriobacteriales</t>
+        </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
           <t>o__Coriobacteriales</t>
         </is>
       </c>
-      <c r="E44" t="inlineStr">
-        <is>
-          <t>o__Coriobacteriales</t>
-        </is>
+      <c r="E44" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="45">
@@ -1459,18 +1459,18 @@
       <c r="B45" t="n">
         <v>129798.0271250198</v>
       </c>
-      <c r="C45" t="n">
-        <v>129798.0271250198</v>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>o__Coriobacteriales</t>
+        </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
           <t>o__Coriobacteriales</t>
         </is>
       </c>
-      <c r="E45" t="inlineStr">
-        <is>
-          <t>o__Coriobacteriales</t>
-        </is>
+      <c r="E45" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="46">
@@ -1482,18 +1482,18 @@
       <c r="B46" t="n">
         <v>132051.0258499979</v>
       </c>
-      <c r="C46" t="n">
-        <v>132051.0258499979</v>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>o__Coriobacteriales</t>
+        </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
           <t>o__Coriobacteriales</t>
         </is>
       </c>
-      <c r="E46" t="inlineStr">
-        <is>
-          <t>o__Coriobacteriales</t>
-        </is>
+      <c r="E46" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="47">
@@ -1505,18 +1505,18 @@
       <c r="B47" t="n">
         <v>86545.42685853491</v>
       </c>
-      <c r="C47" t="n">
-        <v>86545.42685853491</v>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>o__Coriobacteriales</t>
+        </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
           <t>o__Coriobacteriales</t>
         </is>
       </c>
-      <c r="E47" t="inlineStr">
-        <is>
-          <t>o__Coriobacteriales</t>
-        </is>
+      <c r="E47" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="48">
@@ -1528,18 +1528,18 @@
       <c r="B48" t="n">
         <v>47480.13237346197</v>
       </c>
-      <c r="C48" t="n">
-        <v>47480.13237346197</v>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>o__Coriobacteriales</t>
+        </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
           <t>o__Coriobacteriales</t>
         </is>
       </c>
-      <c r="E48" t="inlineStr">
-        <is>
-          <t>o__Coriobacteriales</t>
-        </is>
+      <c r="E48" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="49">
@@ -1551,18 +1551,18 @@
       <c r="B49" t="n">
         <v>41531.70534626418</v>
       </c>
-      <c r="C49" t="n">
-        <v>41531.70534626418</v>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>o__Coriobacteriales</t>
+        </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
           <t>o__Coriobacteriales</t>
         </is>
       </c>
-      <c r="E49" t="inlineStr">
-        <is>
-          <t>o__Coriobacteriales</t>
-        </is>
+      <c r="E49" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="50">
@@ -1574,18 +1574,18 @@
       <c r="B50" t="n">
         <v>72804.58611818566</v>
       </c>
-      <c r="C50" t="n">
-        <v>72804.58611818566</v>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>o__Coriobacteriales</t>
+        </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
           <t>o__Coriobacteriales</t>
         </is>
       </c>
-      <c r="E50" t="inlineStr">
-        <is>
-          <t>o__Coriobacteriales</t>
-        </is>
+      <c r="E50" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="51">
@@ -1597,18 +1597,18 @@
       <c r="B51" t="n">
         <v>122419.1964913189</v>
       </c>
-      <c r="C51" t="n">
-        <v>122419.1964913189</v>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>o__Coriobacteriales</t>
+        </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
           <t>o__Coriobacteriales</t>
         </is>
       </c>
-      <c r="E51" t="inlineStr">
-        <is>
-          <t>o__Coriobacteriales</t>
-        </is>
+      <c r="E51" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="52">
@@ -1620,18 +1620,18 @@
       <c r="B52" t="n">
         <v>93016.55630562179</v>
       </c>
-      <c r="C52" t="n">
-        <v>93016.55630562179</v>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>o__Coriobacteriales</t>
+        </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
           <t>o__Coriobacteriales</t>
         </is>
       </c>
-      <c r="E52" t="inlineStr">
-        <is>
-          <t>o__Coriobacteriales</t>
-        </is>
+      <c r="E52" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="53">
@@ -1643,18 +1643,18 @@
       <c r="B53" t="n">
         <v>24209.42494731227</v>
       </c>
-      <c r="C53" t="n">
-        <v>24209.42494731227</v>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>o__Coriobacteriales</t>
+        </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
           <t>o__Coriobacteriales</t>
         </is>
       </c>
-      <c r="E53" t="inlineStr">
-        <is>
-          <t>o__Coriobacteriales</t>
-        </is>
+      <c r="E53" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="54">
@@ -1666,18 +1666,18 @@
       <c r="B54" t="n">
         <v>23762.80469353742</v>
       </c>
-      <c r="C54" t="n">
-        <v>23762.80469353742</v>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>o__Coriobacteriales</t>
+        </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
           <t>o__Coriobacteriales</t>
         </is>
       </c>
-      <c r="E54" t="inlineStr">
-        <is>
-          <t>o__Coriobacteriales</t>
-        </is>
+      <c r="E54" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="55">
@@ -1689,18 +1689,18 @@
       <c r="B55" t="n">
         <v>90221.4230885257</v>
       </c>
-      <c r="C55" t="n">
-        <v>90221.4230885257</v>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>o__Coriobacteriales</t>
+        </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
           <t>o__Coriobacteriales</t>
         </is>
       </c>
-      <c r="E55" t="inlineStr">
-        <is>
-          <t>o__Coriobacteriales</t>
-        </is>
+      <c r="E55" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="56">
@@ -1712,18 +1712,18 @@
       <c r="B56" t="n">
         <v>95468.63816950354</v>
       </c>
-      <c r="C56" t="n">
-        <v>95468.63816950354</v>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>o__Coriobacteriales</t>
+        </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
           <t>o__Coriobacteriales</t>
         </is>
       </c>
-      <c r="E56" t="inlineStr">
-        <is>
-          <t>o__Coriobacteriales</t>
-        </is>
+      <c r="E56" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>